<commit_message>
Update Sprint 1 Backlog Burndown.xlsx
Re updated the burndown chart after fixing a merge conflict.
</commit_message>
<xml_diff>
--- a/sprints/sprint1/Sprint 1 Backlog Burndown.xlsx
+++ b/sprints/sprint1/Sprint 1 Backlog Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eo00037\source\repos\CapstoneGroup3\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2025 Files\CS 4682 Computing Capstone\CapstoneGroup3\sprints\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFCF845-1BF8-4740-9609-3085C636F50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1138748-69A9-4A57-B135-29C1FE91CDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="10776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,13 +543,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1599,20 +1599,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="151.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.36328125" customWidth="1"/>
+    <col min="2" max="2" width="151.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1650,7 +1650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -1672,7 +1672,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>36</v>
@@ -1714,7 +1714,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>37</v>
@@ -1734,7 +1734,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1744,7 +1744,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
@@ -1754,13 +1754,19 @@
       <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
         <v>35</v>
@@ -1768,13 +1774,15 @@
       <c r="C9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1784,7 +1792,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
@@ -1802,7 +1810,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
         <v>26</v>
@@ -1818,7 +1826,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1828,7 +1836,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
@@ -1850,7 +1858,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>29</v>
@@ -1866,7 +1874,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1876,7 +1884,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1886,13 +1894,19 @@
       <c r="C17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="13" t="s">
         <v>31</v>
@@ -1900,13 +1914,19 @@
       <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="D18" s="5">
+        <v>6</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0</v>
+      </c>
+      <c r="F18" s="9">
+        <v>8</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="20" t="s">
         <v>32</v>
@@ -1918,7 +1938,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="21" t="s">
         <v>33</v>
@@ -1930,7 +1950,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="15"/>
@@ -1940,7 +1960,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1978,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1974,7 +1994,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1984,7 +2004,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1994,7 +2014,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="19" t="s">
         <v>11</v>
@@ -2006,7 +2026,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
         <v>12</v>
@@ -2014,15 +2034,15 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1">
         <f>SUM(D3:D26)</f>
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" ref="E27:H27" si="0">SUM(E3:E26)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
@@ -2048,6 +2068,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B208BF211488B4F880DF934C5C83A74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea6ebcb2e074b139db49da06cf4ed1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71b55cd54d0ee2f4121790f6a497c1d7" ns2:_="">
     <xsd:import namespace="bb8530a4-d58a-4eb7-b41a-d2b9ee1ee59d"/>
@@ -2191,12 +2217,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2207,6 +2227,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D5C3914-7DAF-4B4D-BA97-A88E18DCB9DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2224,15 +2253,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9195D0-9C19-4815-A26D-A7BB393C0F0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A4F540-0AB9-43E5-9CA4-0E2ADF00CD9E}">
   <ds:schemaRefs>

</xml_diff>